<commit_message>
Daily Status Xl Sheet Has been updated
</commit_message>
<xml_diff>
--- a/documents/daily_status.xlsx
+++ b/documents/daily_status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Training Student Name" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="523">
   <si>
     <t xml:space="preserve">Name Of Student </t>
   </si>
@@ -3896,9 +3896,6 @@
     <t>Card Board Cutting</t>
   </si>
   <si>
-    <t>PVC Tape</t>
-  </si>
-  <si>
     <t>Tape</t>
   </si>
   <si>
@@ -3948,6 +3945,21 @@
   </si>
   <si>
     <t>Tabbaco Tracking Asp.net</t>
+  </si>
+  <si>
+    <t>13th feb 2015</t>
+  </si>
+  <si>
+    <t>Anmol singh</t>
+  </si>
+  <si>
+    <t>Soldering</t>
+  </si>
+  <si>
+    <t>13th Feb</t>
+  </si>
+  <si>
+    <t>sushant</t>
   </si>
 </sst>
 </file>
@@ -4675,8 +4687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4799,10 +4811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5287,25 +5299,59 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B20">
         <v>8375940733</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F20">
         <v>400</v>
       </c>
       <c r="H20" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>519</v>
+      </c>
+      <c r="B21">
+        <v>9838195681</v>
+      </c>
+      <c r="D21" t="s">
+        <v>520</v>
+      </c>
+      <c r="E21" t="s">
+        <v>521</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>522</v>
+      </c>
+      <c r="B22">
+        <v>9793382456</v>
+      </c>
+      <c r="D22" t="s">
+        <v>520</v>
+      </c>
+      <c r="E22" t="s">
+        <v>521</v>
+      </c>
+      <c r="F22">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -5334,7 +5380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -5631,19 +5677,19 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B16">
         <v>7042248420</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="D16" t="s">
         <v>516</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>517</v>
-      </c>
-      <c r="E16" t="s">
-        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -5670,48 +5716,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B2" t="s">
         <v>510</v>
-      </c>
-      <c r="B2" t="s">
-        <v>511</v>
       </c>
       <c r="C2">
         <v>31253</v>
@@ -5724,6 +5770,20 @@
       </c>
       <c r="F2">
         <v>1990</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" t="s">
+        <v>518</v>
+      </c>
+      <c r="C3">
+        <v>3080</v>
+      </c>
+      <c r="E3">
+        <v>5049</v>
+      </c>
+      <c r="F3">
+        <v>5070</v>
       </c>
     </row>
   </sheetData>
@@ -5735,8 +5795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5992,10 +6052,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>498</v>
+      </c>
+      <c r="B23" t="s">
         <v>501</v>
-      </c>
-      <c r="B23" t="s">
-        <v>502</v>
       </c>
       <c r="C23">
         <v>50</v>
@@ -7018,7 +7078,7 @@
         <v>6000</v>
       </c>
       <c r="I3" s="81" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J3" s="81"/>
       <c r="K3" s="85" t="s">

</xml_diff>

<commit_message>
Daily Status Has been updated
</commit_message>
<xml_diff>
--- a/documents/daily_status.xlsx
+++ b/documents/daily_status.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7965" tabRatio="815" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Training Student Name" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="594">
   <si>
     <t xml:space="preserve">Name Of Student </t>
   </si>
@@ -4133,12 +4133,54 @@
   <si>
     <t xml:space="preserve">Track the requirements and delivery of projects </t>
   </si>
+  <si>
+    <t>Vipin</t>
+  </si>
+  <si>
+    <t>vipinchauhan247@gmail.com</t>
+  </si>
+  <si>
+    <t>Multi purpose Electronic</t>
+  </si>
+  <si>
+    <t>18th Feb</t>
+  </si>
+  <si>
+    <t>Variable wind power plant</t>
+  </si>
+  <si>
+    <t>sohanshine@gmail.com</t>
+  </si>
+  <si>
+    <t>9136791828</t>
+  </si>
+  <si>
+    <t>Within 1 Month</t>
+  </si>
+  <si>
+    <t>18th feb 2015</t>
+  </si>
+  <si>
+    <t>Prakash Pandey</t>
+  </si>
+  <si>
+    <t>luckyprakash021@gmail.com</t>
+  </si>
+  <si>
+    <t>G.N.I.O.T</t>
+  </si>
+  <si>
+    <t>18th feb</t>
+  </si>
+  <si>
+    <t>Carbon Paper</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4384,7 +4426,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4601,6 +4643,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4663,7 +4708,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4695,10 +4740,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4730,7 +4774,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4906,14 +4949,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
@@ -4927,7 +4970,7 @@
     <col min="11" max="11" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4959,7 +5002,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="75" customFormat="1">
       <c r="A2" s="75" t="s">
         <v>6</v>
       </c>
@@ -4991,7 +5034,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -5023,7 +5066,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>528</v>
       </c>
@@ -5046,7 +5089,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>529</v>
       </c>
@@ -5069,7 +5112,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>545</v>
       </c>
@@ -5095,7 +5138,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>549</v>
       </c>
@@ -5121,7 +5164,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>551</v>
       </c>
@@ -5147,7 +5190,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>554</v>
       </c>
@@ -5187,14 +5230,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
@@ -5207,7 +5250,7 @@
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5233,7 +5276,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -5259,7 +5302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5282,7 +5325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -5308,7 +5351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -5334,7 +5377,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -5360,7 +5403,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -5383,7 +5426,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -5406,7 +5449,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -5432,7 +5475,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>329</v>
       </c>
@@ -5458,7 +5501,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>332</v>
       </c>
@@ -5484,7 +5527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="71" customFormat="1">
       <c r="A12" s="71" t="s">
         <v>335</v>
       </c>
@@ -5507,7 +5550,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>346</v>
       </c>
@@ -5533,7 +5576,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>363</v>
       </c>
@@ -5559,7 +5602,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="75" customFormat="1">
       <c r="A15" s="75" t="s">
         <v>34</v>
       </c>
@@ -5585,7 +5628,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="77" customFormat="1">
       <c r="A16" s="77" t="s">
         <v>421</v>
       </c>
@@ -5614,7 +5657,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>429</v>
       </c>
@@ -5640,7 +5683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>435</v>
       </c>
@@ -5657,7 +5700,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="B19">
         <v>9711307405</v>
       </c>
@@ -5674,7 +5717,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>502</v>
       </c>
@@ -5697,7 +5740,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>519</v>
       </c>
@@ -5714,7 +5757,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>522</v>
       </c>
@@ -5729,6 +5772,29 @@
       </c>
       <c r="F22">
         <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>580</v>
+      </c>
+      <c r="B23">
+        <v>9654033937</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D23" t="s">
+        <v>582</v>
+      </c>
+      <c r="E23" t="s">
+        <v>583</v>
+      </c>
+      <c r="F23">
+        <v>800</v>
+      </c>
+      <c r="G23">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -5747,21 +5813,22 @@
     <hyperlink ref="C16" r:id="rId12"/>
     <hyperlink ref="C17" r:id="rId13"/>
     <hyperlink ref="C20" r:id="rId14"/>
+    <hyperlink ref="C23" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
@@ -5770,7 +5837,7 @@
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -5790,7 +5857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -5810,7 +5877,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -5830,7 +5897,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -5850,7 +5917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5870,7 +5937,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -5890,7 +5957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -5910,7 +5977,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>358</v>
       </c>
@@ -5930,7 +5997,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>408</v>
       </c>
@@ -5950,7 +6017,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>441</v>
       </c>
@@ -5967,7 +6034,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>445</v>
       </c>
@@ -5984,7 +6051,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>465</v>
       </c>
@@ -6001,7 +6068,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>483</v>
       </c>
@@ -6018,7 +6085,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>492</v>
       </c>
@@ -6035,7 +6102,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>496</v>
       </c>
@@ -6052,7 +6119,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>514</v>
       </c>
@@ -6069,7 +6136,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>540</v>
       </c>
@@ -6084,6 +6151,23 @@
       </c>
       <c r="E17" t="s">
         <v>542</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>589</v>
+      </c>
+      <c r="B18">
+        <v>8130283991</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D18" t="s">
+        <v>591</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -6104,20 +6188,21 @@
     <hyperlink ref="C15" r:id="rId14"/>
     <hyperlink ref="C16" r:id="rId15"/>
     <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.7109375" style="94" customWidth="1"/>
     <col min="2" max="2" width="15" style="96" customWidth="1"/>
@@ -6126,7 +6211,7 @@
     <col min="5" max="5" width="13.85546875" style="97" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="61" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="61" customFormat="1">
       <c r="A1" s="92" t="s">
         <v>561</v>
       </c>
@@ -6143,7 +6228,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="94" t="s">
         <v>566</v>
       </c>
@@ -6160,7 +6245,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="94" t="s">
         <v>569</v>
       </c>
@@ -6177,7 +6262,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="94" t="s">
         <v>570</v>
       </c>
@@ -6194,7 +6279,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45">
       <c r="A5" s="94" t="s">
         <v>571</v>
       </c>
@@ -6211,7 +6296,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45">
       <c r="A6" s="94" t="s">
         <v>572</v>
       </c>
@@ -6228,7 +6313,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45">
       <c r="A7" s="94" t="s">
         <v>573</v>
       </c>
@@ -6245,7 +6330,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="94" t="s">
         <v>574</v>
       </c>
@@ -6262,7 +6347,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="94" t="s">
         <v>575</v>
       </c>
@@ -6279,7 +6364,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="94" t="s">
         <v>576</v>
       </c>
@@ -6296,7 +6381,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="94" t="s">
         <v>577</v>
       </c>
@@ -6313,7 +6398,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="94" t="s">
         <v>578</v>
       </c>
@@ -6330,7 +6415,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="94" t="s">
         <v>579</v>
       </c>
@@ -6354,14 +6439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
@@ -6371,7 +6456,7 @@
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>506</v>
       </c>
@@ -6391,7 +6476,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>509</v>
       </c>
@@ -6411,7 +6496,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>518</v>
       </c>
@@ -6425,7 +6510,7 @@
         <v>5070</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>532</v>
       </c>
@@ -6439,7 +6524,7 @@
         <v>10070</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>532</v>
       </c>
@@ -6450,13 +6535,13 @@
         <v>10000</v>
       </c>
       <c r="E5">
-        <v>10049</v>
+        <v>1049</v>
       </c>
       <c r="F5">
         <v>1070</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>559</v>
       </c>
@@ -6464,13 +6549,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>10049</v>
+        <v>1049</v>
       </c>
       <c r="F6">
         <v>1070</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>560</v>
       </c>
@@ -6478,10 +6563,27 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>10049</v>
+        <v>1049</v>
       </c>
       <c r="F7">
         <v>1070</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>588</v>
+      </c>
+      <c r="C8">
+        <v>2300</v>
+      </c>
+      <c r="D8">
+        <v>735</v>
+      </c>
+      <c r="E8">
+        <v>2614</v>
+      </c>
+      <c r="F8">
+        <v>2635</v>
       </c>
     </row>
   </sheetData>
@@ -6490,14 +6592,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
@@ -6506,7 +6608,7 @@
     <col min="5" max="6" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -6517,7 +6619,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -6528,7 +6630,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -6539,7 +6641,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -6550,7 +6652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -6561,7 +6663,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>338</v>
       </c>
@@ -6572,7 +6674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>338</v>
       </c>
@@ -6583,7 +6685,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>338</v>
       </c>
@@ -6594,7 +6696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>338</v>
       </c>
@@ -6605,7 +6707,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>348</v>
       </c>
@@ -6616,7 +6718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>348</v>
       </c>
@@ -6627,7 +6729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>419</v>
       </c>
@@ -6638,7 +6740,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>427</v>
       </c>
@@ -6649,7 +6751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>437</v>
       </c>
@@ -6660,7 +6762,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>437</v>
       </c>
@@ -6671,7 +6773,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>437</v>
       </c>
@@ -6682,7 +6784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>448</v>
       </c>
@@ -6693,7 +6795,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>449</v>
       </c>
@@ -6704,7 +6806,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>488</v>
       </c>
@@ -6715,7 +6817,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>488</v>
       </c>
@@ -6726,7 +6828,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>498</v>
       </c>
@@ -6737,7 +6839,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>498</v>
       </c>
@@ -6748,7 +6850,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>498</v>
       </c>
@@ -6759,7 +6861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>534</v>
       </c>
@@ -6770,7 +6872,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>543</v>
       </c>
@@ -6779,6 +6881,28 @@
       </c>
       <c r="C25">
         <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>592</v>
+      </c>
+      <c r="B26" t="s">
+        <v>450</v>
+      </c>
+      <c r="C26">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>592</v>
+      </c>
+      <c r="B27" t="s">
+        <v>593</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6787,19 +6911,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -6807,7 +6931,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -6815,7 +6939,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -6823,7 +6947,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -6831,7 +6955,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -6839,7 +6963,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -6847,7 +6971,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -6855,7 +6979,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -6863,7 +6987,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -6871,7 +6995,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -6879,7 +7003,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -6887,7 +7011,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -6895,7 +7019,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -6903,7 +7027,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>345</v>
       </c>
@@ -6911,7 +7035,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>368</v>
       </c>
@@ -6919,7 +7043,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>369</v>
       </c>
@@ -6927,7 +7051,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>370</v>
       </c>
@@ -6935,7 +7059,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -6943,7 +7067,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>377</v>
       </c>
@@ -6951,7 +7075,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>383</v>
       </c>
@@ -6959,7 +7083,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>388</v>
       </c>
@@ -6967,7 +7091,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>389</v>
       </c>
@@ -6975,7 +7099,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>390</v>
       </c>
@@ -6983,7 +7107,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -6991,7 +7115,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>460</v>
       </c>
@@ -6999,7 +7123,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>461</v>
       </c>
@@ -7007,7 +7131,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>462</v>
       </c>
@@ -7021,15 +7145,15 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="11"/>
     <col min="2" max="2" width="27.7109375" style="12" customWidth="1"/>
@@ -7739,7 +7863,7 @@
     <col min="16140" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="10" customFormat="1" ht="25.5">
       <c r="A1" s="5" t="s">
         <v>89</v>
       </c>
@@ -7775,8 +7899,8 @@
       </c>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:12" s="86" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="13.5" thickBot="1"/>
+    <row r="3" spans="1:12" s="86" customFormat="1" ht="13.5" thickBot="1">
       <c r="A3" s="80">
         <v>1</v>
       </c>
@@ -7806,7 +7930,7 @@
       </c>
       <c r="L3" s="85"/>
     </row>
-    <row r="4" spans="1:12" s="70" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="70" customFormat="1" ht="26.25" thickBot="1">
       <c r="A4" s="63">
         <v>2</v>
       </c>
@@ -7838,7 +7962,7 @@
       </c>
       <c r="L4" s="69"/>
     </row>
-    <row r="5" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1">
       <c r="A5" s="31">
         <v>3</v>
       </c>
@@ -7870,7 +7994,7 @@
       </c>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="1:12" s="30" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="30" customFormat="1" ht="13.5" thickBot="1">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -7902,7 +8026,7 @@
       </c>
       <c r="L6" s="29"/>
     </row>
-    <row r="7" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1">
       <c r="A7" s="31">
         <v>5</v>
       </c>
@@ -7934,7 +8058,7 @@
       </c>
       <c r="L7" s="38"/>
     </row>
-    <row r="8" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
       <c r="A8" s="31">
         <v>6</v>
       </c>
@@ -7966,7 +8090,7 @@
       </c>
       <c r="L8" s="38"/>
     </row>
-    <row r="9" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1">
       <c r="A9" s="31">
         <v>7</v>
       </c>
@@ -7996,7 +8120,7 @@
       </c>
       <c r="L9" s="38"/>
     </row>
-    <row r="10" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="39" customFormat="1" ht="13.5" thickBot="1">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -8026,7 +8150,7 @@
       </c>
       <c r="L10" s="38"/>
     </row>
-    <row r="11" spans="1:12" s="39" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="39" customFormat="1" ht="39" thickBot="1">
       <c r="A11" s="31">
         <v>9</v>
       </c>
@@ -8060,7 +8184,7 @@
       </c>
       <c r="L11" s="38"/>
     </row>
-    <row r="12" spans="1:12" s="30" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="30" customFormat="1" ht="51.75" thickBot="1">
       <c r="A12" s="23">
         <v>10</v>
       </c>
@@ -8092,7 +8216,7 @@
       </c>
       <c r="L12" s="29"/>
     </row>
-    <row r="13" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1">
       <c r="A13" s="16">
         <v>11</v>
       </c>
@@ -8124,7 +8248,7 @@
       </c>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="22" customFormat="1" ht="26.25" thickBot="1">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -8156,7 +8280,7 @@
       </c>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:12" s="30" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="30" customFormat="1" ht="26.25" thickBot="1">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -8188,7 +8312,7 @@
       </c>
       <c r="L15" s="29"/>
     </row>
-    <row r="16" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
       <c r="A16" s="31">
         <v>15</v>
       </c>
@@ -8216,7 +8340,7 @@
       </c>
       <c r="L16" s="38"/>
     </row>
-    <row r="17" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
       <c r="A17" s="31">
         <v>16</v>
       </c>
@@ -8248,7 +8372,7 @@
       </c>
       <c r="L17" s="38"/>
     </row>
-    <row r="18" spans="1:12" s="47" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="47" customFormat="1" ht="26.25" thickBot="1">
       <c r="A18" s="43">
         <v>17</v>
       </c>
@@ -8282,7 +8406,7 @@
       </c>
       <c r="L18" s="46"/>
     </row>
-    <row r="19" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="39" customFormat="1" ht="26.25" thickBot="1">
       <c r="A19" s="31">
         <v>19</v>
       </c>
@@ -8314,7 +8438,7 @@
       </c>
       <c r="L19" s="38"/>
     </row>
-    <row r="20" spans="1:12" s="52" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="52" customFormat="1" ht="30.75" thickBot="1">
       <c r="A20" s="48">
         <v>20</v>
       </c>
@@ -8346,7 +8470,7 @@
       <c r="K20" s="50"/>
       <c r="L20" s="51"/>
     </row>
-    <row r="21" spans="1:12" s="52" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="52" customFormat="1" ht="30.75" thickBot="1">
       <c r="A21" s="48">
         <v>21</v>
       </c>
@@ -8379,27 +8503,60 @@
         <v>539</v>
       </c>
       <c r="L21" s="51"/>
+    </row>
+    <row r="22" spans="1:12" ht="30">
+      <c r="A22" s="11">
+        <v>22</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="98" t="s">
+        <v>585</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="H22" s="11">
+        <v>3000</v>
+      </c>
+      <c r="I22" s="11">
+        <v>1000</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>587</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E18" r:id="rId1"/>
     <hyperlink ref="E20" r:id="rId2"/>
     <hyperlink ref="E21" r:id="rId3"/>
+    <hyperlink ref="E22" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A231" sqref="A231"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="84.85546875" style="59" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="15" customWidth="1"/>
@@ -8407,7 +8564,7 @@
     <col min="4" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="18">
       <c r="A1" s="53" t="s">
         <v>152</v>
       </c>
@@ -8421,13 +8578,13 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="54"/>
       <c r="D2" s="15">
         <v>1800</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16.5">
       <c r="A3" s="55" t="s">
         <v>155</v>
       </c>
@@ -8435,7 +8592,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="56" t="s">
         <v>156</v>
       </c>
@@ -8446,7 +8603,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="54" t="s">
         <v>157</v>
       </c>
@@ -8457,7 +8614,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="54" t="s">
         <v>158</v>
       </c>
@@ -8468,7 +8625,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="54" t="s">
         <v>159</v>
       </c>
@@ -8479,7 +8636,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="54" t="s">
         <v>160</v>
       </c>
@@ -8490,7 +8647,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="54" t="s">
         <v>161</v>
       </c>
@@ -8501,7 +8658,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="56" t="s">
         <v>162</v>
       </c>
@@ -8512,7 +8669,7 @@
         <v>5800</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="54" t="s">
         <v>163</v>
       </c>
@@ -8523,7 +8680,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" s="54" t="s">
         <v>164</v>
       </c>
@@ -8534,12 +8691,12 @@
         <v>6800</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15">
       <c r="A13" s="57" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15">
       <c r="A14" s="54" t="s">
         <v>166</v>
       </c>
@@ -8547,7 +8704,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15">
       <c r="A15" s="54" t="s">
         <v>167</v>
       </c>
@@ -8555,7 +8712,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15">
       <c r="A16" s="54" t="s">
         <v>168</v>
       </c>
@@ -8563,12 +8720,12 @@
         <v>910</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="57" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="56" t="s">
         <v>170</v>
       </c>
@@ -8576,7 +8733,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="54" t="s">
         <v>171</v>
       </c>
@@ -8584,7 +8741,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" s="54" t="s">
         <v>172</v>
       </c>
@@ -8592,7 +8749,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="54" t="s">
         <v>173</v>
       </c>
@@ -8600,7 +8757,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="54" t="s">
         <v>174</v>
       </c>
@@ -8608,7 +8765,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="54" t="s">
         <v>175</v>
       </c>
@@ -8616,7 +8773,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15">
       <c r="A24" s="54" t="s">
         <v>176</v>
       </c>
@@ -8624,7 +8781,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A25" s="73" t="s">
         <v>381</v>
       </c>
@@ -8632,7 +8789,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="54" t="s">
         <v>344</v>
       </c>
@@ -8640,7 +8797,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A27" s="73" t="s">
         <v>349</v>
       </c>
@@ -8648,7 +8805,7 @@
         <v>2041</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A28" s="73" t="s">
         <v>350</v>
       </c>
@@ -8656,7 +8813,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A29" s="73" t="s">
         <v>351</v>
       </c>
@@ -8664,7 +8821,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A30" s="73" t="s">
         <v>382</v>
       </c>
@@ -8672,17 +8829,17 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A31" s="57" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A32" s="57" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A33" s="57" t="s">
         <v>366</v>
       </c>
@@ -8690,7 +8847,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="15">
       <c r="A34" s="54" t="s">
         <v>367</v>
       </c>
@@ -8698,17 +8855,17 @@
         <v>682</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A35" s="57" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A36" s="57" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" s="54" t="s">
         <v>371</v>
       </c>
@@ -8716,7 +8873,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="15">
       <c r="A38" s="54" t="s">
         <v>373</v>
       </c>
@@ -8724,7 +8881,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="15">
       <c r="A39" s="54" t="s">
         <v>374</v>
       </c>
@@ -8732,7 +8889,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="15">
       <c r="A40" s="54" t="s">
         <v>375</v>
       </c>
@@ -8740,7 +8897,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="15">
       <c r="A41" s="54" t="s">
         <v>376</v>
       </c>
@@ -8748,7 +8905,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A42" s="73" t="s">
         <v>384</v>
       </c>
@@ -8756,12 +8913,12 @@
         <v>2365</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A43" s="57" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A44" s="73" t="s">
         <v>385</v>
       </c>
@@ -8769,7 +8926,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="15">
       <c r="A45" s="54" t="s">
         <v>182</v>
       </c>
@@ -8777,12 +8934,12 @@
         <v>936</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A46" s="57" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="15">
       <c r="A47" s="54" t="s">
         <v>378</v>
       </c>
@@ -8790,141 +8947,141 @@
         <v>575</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="15">
       <c r="A48" s="58"/>
     </row>
-    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" ht="15">
       <c r="A49" s="54"/>
     </row>
-    <row r="50" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="16.5">
       <c r="A50" s="55" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" ht="15">
       <c r="A51" s="54" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" ht="15">
       <c r="A52" s="54" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" ht="15">
       <c r="A53" s="54" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" ht="15">
       <c r="A54" s="54" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" ht="15">
       <c r="A55" s="54" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" ht="15">
       <c r="A56" s="54" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" ht="15">
       <c r="A57" s="54" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" ht="15">
       <c r="A58" s="54" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" ht="15">
       <c r="A59" s="54" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" ht="15">
       <c r="A60" s="54" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" ht="15">
       <c r="A61" s="54" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" ht="15">
       <c r="A62" s="54" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" ht="15">
       <c r="A63" s="54" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" ht="15">
       <c r="A64" s="54" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="15">
       <c r="A65" s="54" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="15">
       <c r="A66" s="54" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="15">
       <c r="A67" s="54" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="15">
       <c r="A68" s="54" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="15">
       <c r="A69" s="54" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="15">
       <c r="A70" s="54" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="15">
       <c r="A71" s="54" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="15">
       <c r="A72" s="54" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="15">
       <c r="A73" s="54" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="15">
       <c r="A74" s="54"/>
     </row>
-    <row r="75" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="16.5">
       <c r="A75" s="55" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="15">
       <c r="A76" s="54" t="s">
         <v>209</v>
       </c>
@@ -8932,7 +9089,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="15">
       <c r="A77" s="54" t="s">
         <v>391</v>
       </c>
@@ -8940,7 +9097,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="15">
       <c r="A78" s="54" t="s">
         <v>392</v>
       </c>
@@ -8948,7 +9105,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="15">
       <c r="A79" s="54" t="s">
         <v>210</v>
       </c>
@@ -8956,7 +9113,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="15">
       <c r="A80" s="54" t="s">
         <v>393</v>
       </c>
@@ -8964,7 +9121,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="15">
       <c r="A81" s="54" t="s">
         <v>211</v>
       </c>
@@ -8972,7 +9129,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="15">
       <c r="A82" s="54" t="s">
         <v>394</v>
       </c>
@@ -8980,7 +9137,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="15">
       <c r="A83" s="54" t="s">
         <v>395</v>
       </c>
@@ -8988,12 +9145,12 @@
         <v>936</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A84" s="57" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="15">
       <c r="A85" s="54" t="s">
         <v>396</v>
       </c>
@@ -9001,12 +9158,12 @@
         <v>975</v>
       </c>
     </row>
-    <row r="86" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A86" s="57" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="15">
       <c r="A87" s="54" t="s">
         <v>214</v>
       </c>
@@ -9014,7 +9171,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="15">
       <c r="A88" s="54" t="s">
         <v>397</v>
       </c>
@@ -9022,7 +9179,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="15">
       <c r="A89" s="54" t="s">
         <v>398</v>
       </c>
@@ -9030,7 +9187,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15">
       <c r="A90" s="54" t="s">
         <v>399</v>
       </c>
@@ -9038,7 +9195,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="15">
       <c r="A91" s="54" t="s">
         <v>400</v>
       </c>
@@ -9046,7 +9203,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="15">
       <c r="A92" s="54" t="s">
         <v>401</v>
       </c>
@@ -9054,7 +9211,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="15">
       <c r="A93" s="54" t="s">
         <v>402</v>
       </c>
@@ -9062,12 +9219,12 @@
         <v>910</v>
       </c>
     </row>
-    <row r="94" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A94" s="57" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="15">
       <c r="A95" s="54" t="s">
         <v>403</v>
       </c>
@@ -9075,7 +9232,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="15">
       <c r="A96" s="54" t="s">
         <v>404</v>
       </c>
@@ -9083,7 +9240,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="15">
       <c r="A97" s="54" t="s">
         <v>405</v>
       </c>
@@ -9091,12 +9248,12 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="98" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A98" s="57" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="15">
       <c r="A99" s="54" t="s">
         <v>217</v>
       </c>
@@ -9104,7 +9261,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="15">
       <c r="A100" s="54" t="s">
         <v>406</v>
       </c>
@@ -9112,12 +9269,12 @@
         <v>3475</v>
       </c>
     </row>
-    <row r="101" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A101" s="57" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="15">
       <c r="A102" s="54" t="s">
         <v>407</v>
       </c>
@@ -9125,20 +9282,20 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="15">
       <c r="A103" s="54" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="15">
       <c r="A104" s="54"/>
     </row>
-    <row r="105" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="16.5">
       <c r="A105" s="55" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="15">
       <c r="A106" s="54" t="s">
         <v>415</v>
       </c>
@@ -9146,7 +9303,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="15">
       <c r="A107" s="54" t="s">
         <v>220</v>
       </c>
@@ -9154,7 +9311,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="15">
       <c r="A108" s="54" t="s">
         <v>416</v>
       </c>
@@ -9162,7 +9319,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="15">
       <c r="A109" s="54" t="s">
         <v>417</v>
       </c>
@@ -9170,7 +9327,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="15">
       <c r="A110" s="54" t="s">
         <v>418</v>
       </c>
@@ -9178,7 +9335,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="15">
       <c r="A111" s="54" t="s">
         <v>420</v>
       </c>
@@ -9186,7 +9343,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="15">
       <c r="A112" s="54" t="s">
         <v>221</v>
       </c>
@@ -9194,7 +9351,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="15">
       <c r="A113" s="54" t="s">
         <v>454</v>
       </c>
@@ -9202,7 +9359,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="15">
       <c r="A114" s="54" t="s">
         <v>222</v>
       </c>
@@ -9210,12 +9367,12 @@
         <v>660</v>
       </c>
     </row>
-    <row r="115" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A115" s="57" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="15">
       <c r="A116" s="54" t="s">
         <v>224</v>
       </c>
@@ -9223,7 +9380,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="15">
       <c r="A117" s="54" t="s">
         <v>455</v>
       </c>
@@ -9231,7 +9388,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="15">
       <c r="A118" s="54" t="s">
         <v>456</v>
       </c>
@@ -9239,25 +9396,25 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="15">
       <c r="A119" s="54" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" ht="15">
       <c r="A120" s="54"/>
     </row>
-    <row r="121" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="16.5">
       <c r="A121" s="55" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A122" s="57" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="15">
       <c r="A123" s="54" t="s">
         <v>227</v>
       </c>
@@ -9265,7 +9422,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="15">
       <c r="A124" s="54" t="s">
         <v>228</v>
       </c>
@@ -9273,7 +9430,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="15">
       <c r="A125" s="54" t="s">
         <v>229</v>
       </c>
@@ -9281,7 +9438,7 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" ht="15">
       <c r="A126" s="54" t="s">
         <v>230</v>
       </c>
@@ -9289,7 +9446,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" ht="15">
       <c r="A127" s="54" t="s">
         <v>457</v>
       </c>
@@ -9297,37 +9454,37 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="128" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A128" s="57" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="129" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A129" s="57" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="130" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A130" s="57" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="131" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A131" s="57" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="132" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A132" s="57" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="133" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A133" s="57" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="15">
       <c r="A134" s="54" t="s">
         <v>237</v>
       </c>
@@ -9335,42 +9492,42 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="135" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A135" s="57" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="136" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A136" s="57" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="137" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A137" s="57" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="138" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A138" s="57" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" ht="15">
       <c r="A139" s="54" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="140" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A140" s="57" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="141" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A141" s="57" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" ht="15">
       <c r="A142" s="54" t="s">
         <v>245</v>
       </c>
@@ -9378,7 +9535,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" ht="15">
       <c r="A143" s="54" t="s">
         <v>246</v>
       </c>
@@ -9386,45 +9543,45 @@
         <v>2807</v>
       </c>
     </row>
-    <row r="144" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A144" s="57" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="145" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A145" s="57" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="146" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A146" s="57" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="147" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A147" s="57" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="148" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A148" s="57" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="149" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A149" s="57" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="15">
       <c r="A150" s="54"/>
     </row>
-    <row r="151" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="16.5">
       <c r="A151" s="55" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" ht="15">
       <c r="A152" s="54" t="s">
         <v>254</v>
       </c>
@@ -9432,7 +9589,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" ht="15">
       <c r="A153" s="54" t="s">
         <v>255</v>
       </c>
@@ -9440,7 +9597,7 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="15">
       <c r="A154" s="54" t="s">
         <v>256</v>
       </c>
@@ -9448,7 +9605,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="15">
       <c r="A155" s="54" t="s">
         <v>458</v>
       </c>
@@ -9456,7 +9613,7 @@
         <v>3240</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="15">
       <c r="A156" s="54" t="s">
         <v>257</v>
       </c>
@@ -9464,7 +9621,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="15">
       <c r="A157" s="54" t="s">
         <v>459</v>
       </c>
@@ -9472,17 +9629,17 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="15">
       <c r="A158" s="54" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" ht="16.5">
       <c r="A159" s="55" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" ht="15">
       <c r="A160" s="54" t="s">
         <v>259</v>
       </c>
@@ -9490,7 +9647,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" ht="15">
       <c r="A161" s="54" t="s">
         <v>260</v>
       </c>
@@ -9498,17 +9655,17 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="162" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A162" s="57" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="163" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A163" s="57" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="164" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A164" s="57" t="s">
         <v>263</v>
       </c>
@@ -9516,7 +9673,7 @@
         <v>3475</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" ht="15">
       <c r="A165" s="54" t="s">
         <v>264</v>
       </c>
@@ -9524,62 +9681,62 @@
         <v>2360</v>
       </c>
     </row>
-    <row r="166" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A166" s="57" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="167" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A167" s="57" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="168" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A168" s="57" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="169" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A169" s="57" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="170" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A170" s="57" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="171" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A171" s="57" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="172" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A172" s="57" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="173" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A173" s="57" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="174" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A174" s="57" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="175" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A175" s="57" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="176" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A176" s="57" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" ht="15">
       <c r="A177" s="54" t="s">
         <v>276</v>
       </c>
@@ -9587,12 +9744,12 @@
         <v>3190</v>
       </c>
     </row>
-    <row r="178" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A178" s="57" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="15">
       <c r="A179" s="54" t="s">
         <v>469</v>
       </c>
@@ -9600,7 +9757,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" ht="15">
       <c r="A180" s="54" t="s">
         <v>470</v>
       </c>
@@ -9608,12 +9765,12 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="181" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A181" s="57" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" ht="15">
       <c r="A182" s="54" t="s">
         <v>471</v>
       </c>
@@ -9621,17 +9778,17 @@
         <v>2870</v>
       </c>
     </row>
-    <row r="183" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A183" s="57" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="184" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A184" s="57" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" ht="15">
       <c r="A185" s="54" t="s">
         <v>472</v>
       </c>
@@ -9639,55 +9796,55 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="186" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A186" s="57" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="187" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A187" s="57" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="188" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A188" s="57" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="189" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A189" s="57" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="190" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A190" s="57" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="191" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A191" s="57" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="192" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A192" s="57" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="193" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A193" s="57" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" ht="15">
       <c r="A194" s="54"/>
     </row>
-    <row r="195" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" ht="16.5">
       <c r="A195" s="55" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" ht="15">
       <c r="A196" s="54" t="s">
         <v>463</v>
       </c>
@@ -9695,7 +9852,7 @@
         <v>4030</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" ht="15">
       <c r="A197" s="54" t="s">
         <v>290</v>
       </c>
@@ -9703,7 +9860,7 @@
         <v>4280</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" ht="15">
       <c r="A198" s="54" t="s">
         <v>464</v>
       </c>
@@ -9711,7 +9868,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" ht="15">
       <c r="A199" s="54" t="s">
         <v>473</v>
       </c>
@@ -9719,7 +9876,7 @@
         <v>3670</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" ht="15">
       <c r="A200" s="54" t="s">
         <v>474</v>
       </c>
@@ -9727,12 +9884,12 @@
         <v>4280</v>
       </c>
     </row>
-    <row r="201" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A201" s="57" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" ht="15">
       <c r="A202" s="54" t="s">
         <v>475</v>
       </c>
@@ -9740,7 +9897,7 @@
         <v>3865</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" ht="15">
       <c r="A203" s="54" t="s">
         <v>476</v>
       </c>
@@ -9748,7 +9905,7 @@
         <v>3790</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" ht="15">
       <c r="A204" s="54" t="s">
         <v>477</v>
       </c>
@@ -9756,15 +9913,15 @@
         <v>4290</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" ht="15">
       <c r="A205" s="54"/>
     </row>
-    <row r="206" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" ht="16.5">
       <c r="A206" s="55" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" ht="15">
       <c r="A207" s="54" t="s">
         <v>478</v>
       </c>
@@ -9772,7 +9929,7 @@
         <v>3870</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" ht="15">
       <c r="A208" s="54" t="s">
         <v>479</v>
       </c>
@@ -9780,7 +9937,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" ht="15">
       <c r="A209" s="54" t="s">
         <v>480</v>
       </c>
@@ -9788,38 +9945,38 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="210" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A210" s="57" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" ht="15">
       <c r="A211" s="54"/>
     </row>
-    <row r="212" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" ht="16.5">
       <c r="A212" s="55" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" ht="15">
       <c r="A213" s="54" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" ht="15">
       <c r="A214" s="54" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" ht="15">
       <c r="A215" s="54"/>
     </row>
-    <row r="216" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" ht="16.5">
       <c r="A216" s="55" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" ht="15">
       <c r="A217" s="54" t="s">
         <v>481</v>
       </c>
@@ -9827,12 +9984,12 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="218" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A218" s="57" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" ht="15">
       <c r="A219" s="54" t="s">
         <v>482</v>
       </c>
@@ -9840,158 +9997,158 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="220" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A220" s="57" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="221" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A221" s="57" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="222" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A222" s="57" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="223" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A223" s="57" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="224" spans="1:3" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" s="62" customFormat="1" ht="15">
       <c r="A224" s="57" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="225" spans="1:1" s="62" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" s="62" customFormat="1" ht="15">
       <c r="A225" s="57" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="226" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" ht="15">
       <c r="A226" s="54"/>
     </row>
-    <row r="227" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" ht="16.5">
       <c r="A227" s="55" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="228" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" ht="15">
       <c r="A228" s="54" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="229" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" ht="15">
       <c r="A229" s="54"/>
     </row>
-    <row r="230" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" ht="16.5">
       <c r="A230" s="55" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="231" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" ht="15">
       <c r="A231" s="54" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="232" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" ht="15">
       <c r="A232" s="54" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="234" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" ht="16.5">
       <c r="A234" s="55" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1">
       <c r="A235" s="56" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1">
       <c r="A236" s="56" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1">
       <c r="A237" s="56" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1">
       <c r="A238" s="56" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1">
       <c r="A239" s="56" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1">
       <c r="A240" s="56" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="242" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" ht="16.5">
       <c r="A242" s="55" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="244" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" ht="16.5">
       <c r="A244" s="55" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="246" spans="1:1" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" ht="16.5">
       <c r="A246" s="55" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1">
       <c r="A247" s="59" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1">
       <c r="A248" s="59" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1">
       <c r="A249" s="59" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1">
       <c r="A250" s="59" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1">
       <c r="A251" s="59" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1">
       <c r="A252" s="60" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1">
       <c r="A253" s="59" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1">
       <c r="A254" s="59" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1">
       <c r="A255" s="59" t="s">
         <v>328</v>
       </c>

</xml_diff>

<commit_message>
Dailt Atatus xl sheet updated
</commit_message>
<xml_diff>
--- a/documents/daily_status.xlsx
+++ b/documents/daily_status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="7950" tabRatio="815" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="7950" tabRatio="815" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Training Student Name" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,14 @@
     <sheet name="Rate List" sheetId="5" r:id="rId7"/>
     <sheet name="Major Projects Undergoing" sheetId="7" r:id="rId8"/>
     <sheet name="Final Year Projects" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId10"/>
+    <sheet name="Training Weekend And Weekdays" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="652">
   <si>
     <t xml:space="preserve">Name Of Student </t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>8051 With LCD ; Keypad And RS 232</t>
-  </si>
-  <si>
-    <t>RF Module Pcb</t>
   </si>
   <si>
     <t>DC Motor</t>
@@ -4262,13 +4259,103 @@
   </si>
   <si>
     <t>22nd feb 2015</t>
+  </si>
+  <si>
+    <t>sushantkamboj10@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sushant </t>
+  </si>
+  <si>
+    <t>Final year project</t>
+  </si>
+  <si>
+    <t>Ashok kumar</t>
+  </si>
+  <si>
+    <t>ask11shah@gmail.com</t>
+  </si>
+  <si>
+    <t>iimt</t>
+  </si>
+  <si>
+    <t>Emergency light</t>
+  </si>
+  <si>
+    <t>shashank</t>
+  </si>
+  <si>
+    <t>shashank1014@gmail.com</t>
+  </si>
+  <si>
+    <t>RF Module Pcb(self made)</t>
+  </si>
+  <si>
+    <t>RF Module Pcb(Green pcb)</t>
+  </si>
+  <si>
+    <t>Lalit</t>
+  </si>
+  <si>
+    <t>Previous Payment</t>
+  </si>
+  <si>
+    <t>24thFeb</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Weekend</t>
+  </si>
+  <si>
+    <t>Weekdays</t>
+  </si>
+  <si>
+    <t>Hands On</t>
+  </si>
+  <si>
+    <t>Theory</t>
+  </si>
+  <si>
+    <t>Project Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project </t>
+  </si>
+  <si>
+    <t>Practical</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Certificate</t>
+  </si>
+  <si>
+    <t>24nd feb 2015</t>
+  </si>
+  <si>
+    <t>Ashok</t>
+  </si>
+  <si>
+    <t>Street Light</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4337,6 +4424,12 @@
       <color theme="1"/>
       <name val="Wingdings"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -4520,7 +4613,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4760,6 +4853,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5066,8 +5160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5133,19 +5227,19 @@
         <v>7</v>
       </c>
       <c r="F2" s="68" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G2" s="68">
         <v>5000</v>
       </c>
       <c r="H2" s="84" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J2" s="68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K2" s="68" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -5165,33 +5259,33 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G3">
         <v>5000</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B4">
         <v>9971907103</v>
       </c>
       <c r="D4" t="s">
+        <v>527</v>
+      </c>
+      <c r="E4" t="s">
         <v>528</v>
-      </c>
-      <c r="E4" t="s">
-        <v>529</v>
       </c>
       <c r="F4">
         <v>1500</v>
@@ -5200,21 +5294,21 @@
         <v>1500</v>
       </c>
       <c r="H4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B5">
         <v>9971907103</v>
       </c>
       <c r="D5" t="s">
+        <v>527</v>
+      </c>
+      <c r="E5" t="s">
         <v>528</v>
-      </c>
-      <c r="E5" t="s">
-        <v>529</v>
       </c>
       <c r="F5">
         <v>1500</v>
@@ -5223,24 +5317,24 @@
         <v>1500</v>
       </c>
       <c r="H5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B6">
         <v>9911193134</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F6">
         <v>1000</v>
@@ -5249,24 +5343,24 @@
         <v>1500</v>
       </c>
       <c r="H6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B7">
         <v>9643705662</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F7">
         <v>1000</v>
@@ -5275,24 +5369,24 @@
         <v>1500</v>
       </c>
       <c r="H7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B8">
         <v>9899766120</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F8">
         <v>1000</v>
@@ -5301,24 +5395,24 @@
         <v>1500</v>
       </c>
       <c r="H8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B9">
         <v>9650259567</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F9">
         <v>1000</v>
@@ -5327,7 +5421,7 @@
         <v>1500</v>
       </c>
       <c r="H9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -5345,22 +5439,151 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>639</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>565</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>640</v>
+      </c>
+      <c r="B3" s="88" t="s">
+        <v>565</v>
+      </c>
+      <c r="C3" s="88" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>641</v>
+      </c>
+      <c r="B4" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C4" s="88" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>642</v>
+      </c>
+      <c r="B5" s="107">
+        <v>1</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>644</v>
+      </c>
+      <c r="B6" s="88" t="s">
+        <v>565</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>645</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>643</v>
+      </c>
+      <c r="B8" s="88" t="s">
+        <v>565</v>
+      </c>
+      <c r="C8" s="88" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>646</v>
+      </c>
+      <c r="B9" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C9" s="88" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" s="88" t="s">
+        <v>565</v>
+      </c>
+      <c r="C10" s="88" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>648</v>
+      </c>
+      <c r="B11" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C11" s="88" t="s">
+        <v>565</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5393,10 +5616,10 @@
         <v>15</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>449</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>450</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>36</v>
@@ -5577,19 +5800,19 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9">
         <v>9540364146</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F9">
         <v>300</v>
@@ -5603,19 +5826,19 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B10">
         <v>8800934802</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" t="s">
         <v>330</v>
       </c>
-      <c r="D10" t="s">
-        <v>331</v>
-      </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10">
         <v>150</v>
@@ -5629,19 +5852,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B11">
         <v>9971564923</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" t="s">
         <v>333</v>
       </c>
-      <c r="D11" t="s">
-        <v>334</v>
-      </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F11">
         <v>150</v>
@@ -5655,42 +5878,42 @@
     </row>
     <row r="12" spans="1:9" s="64" customFormat="1">
       <c r="A12" s="64" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B12" s="64">
         <v>9871310918</v>
       </c>
       <c r="C12" s="65" t="s">
+        <v>335</v>
+      </c>
+      <c r="D12" s="64" t="s">
         <v>336</v>
       </c>
-      <c r="D12" s="64" t="s">
-        <v>337</v>
-      </c>
       <c r="E12" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="64">
         <v>150</v>
       </c>
       <c r="H12" s="64" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B13">
         <v>9582449984</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F13">
         <v>300</v>
@@ -5704,19 +5927,19 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B14">
         <v>9811708509</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D14" t="s">
         <v>363</v>
       </c>
-      <c r="D14" t="s">
-        <v>364</v>
-      </c>
       <c r="E14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F14">
         <v>100</v>
@@ -5736,13 +5959,13 @@
         <v>9711022937</v>
       </c>
       <c r="C15" s="69" t="s">
+        <v>411</v>
+      </c>
+      <c r="D15" s="68" t="s">
         <v>412</v>
       </c>
-      <c r="D15" s="68" t="s">
-        <v>413</v>
-      </c>
       <c r="E15" s="68" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F15" s="68">
         <v>350</v>
@@ -5756,48 +5979,48 @@
     </row>
     <row r="16" spans="1:9" s="70" customFormat="1">
       <c r="A16" s="70" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B16" s="70">
         <v>9990180164</v>
       </c>
       <c r="C16" s="71" t="s">
+        <v>420</v>
+      </c>
+      <c r="D16" s="70" t="s">
         <v>421</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="E16" s="70" t="s">
         <v>422</v>
-      </c>
-      <c r="E16" s="70" t="s">
-        <v>423</v>
       </c>
       <c r="F16" s="70">
         <v>1500</v>
       </c>
       <c r="G16" s="70" t="s">
+        <v>423</v>
+      </c>
+      <c r="H16" s="70" t="s">
+        <v>423</v>
+      </c>
+      <c r="I16" s="70" t="s">
         <v>424</v>
-      </c>
-      <c r="H16" s="70" t="s">
-        <v>424</v>
-      </c>
-      <c r="I16" s="70" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B17">
         <v>9210036786</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D17" t="s">
+        <v>428</v>
+      </c>
+      <c r="E17" t="s">
         <v>429</v>
-      </c>
-      <c r="E17" t="s">
-        <v>430</v>
       </c>
       <c r="F17">
         <v>250</v>
@@ -5811,13 +6034,13 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
+        <v>433</v>
+      </c>
+      <c r="D18" t="s">
         <v>434</v>
       </c>
-      <c r="D18" t="s">
-        <v>435</v>
-      </c>
       <c r="E18" s="72" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F18">
         <v>20</v>
@@ -5831,10 +6054,10 @@
         <v>9711307405</v>
       </c>
       <c r="D19" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E19" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F19">
         <v>200</v>
@@ -5845,19 +6068,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B20">
         <v>8375940733</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F20">
         <v>400</v>
@@ -5868,16 +6091,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B21">
         <v>9838195681</v>
       </c>
       <c r="D21" t="s">
+        <v>517</v>
+      </c>
+      <c r="E21" t="s">
         <v>518</v>
-      </c>
-      <c r="E21" t="s">
-        <v>519</v>
       </c>
       <c r="F21">
         <v>50</v>
@@ -5888,16 +6111,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B22">
         <v>9793382456</v>
       </c>
       <c r="D22" t="s">
+        <v>517</v>
+      </c>
+      <c r="E22" t="s">
         <v>518</v>
-      </c>
-      <c r="E22" t="s">
-        <v>519</v>
       </c>
       <c r="F22">
         <v>30</v>
@@ -5908,19 +6131,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B23">
         <v>9654033937</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="D23" t="s">
         <v>579</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>580</v>
-      </c>
-      <c r="E23" t="s">
-        <v>581</v>
       </c>
       <c r="F23">
         <v>800</v>
@@ -5934,19 +6157,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B24">
         <v>7053362994</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="D24" t="s">
         <v>593</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>594</v>
-      </c>
-      <c r="E24" t="s">
-        <v>595</v>
       </c>
       <c r="F24">
         <v>400</v>
@@ -5957,19 +6180,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B25">
         <v>8826582906</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="D25" t="s">
         <v>600</v>
       </c>
-      <c r="D25" t="s">
-        <v>601</v>
-      </c>
       <c r="E25" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F25">
         <v>600</v>
@@ -5983,16 +6206,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B26">
         <v>9793382956</v>
       </c>
       <c r="D26" t="s">
+        <v>612</v>
+      </c>
+      <c r="E26" t="s">
         <v>613</v>
-      </c>
-      <c r="E26" t="s">
-        <v>614</v>
       </c>
       <c r="F26">
         <v>600</v>
@@ -6001,6 +6224,52 @@
         <v>600</v>
       </c>
       <c r="H26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>633</v>
+      </c>
+      <c r="B27">
+        <v>9718155292</v>
+      </c>
+      <c r="D27" t="s">
+        <v>634</v>
+      </c>
+      <c r="E27" t="s">
+        <v>635</v>
+      </c>
+      <c r="F27">
+        <v>2000</v>
+      </c>
+      <c r="G27">
+        <v>2000</v>
+      </c>
+      <c r="H27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>650</v>
+      </c>
+      <c r="B28">
+        <v>8750546916</v>
+      </c>
+      <c r="D28" t="s">
+        <v>651</v>
+      </c>
+      <c r="E28" t="s">
+        <v>635</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>50</v>
+      </c>
+      <c r="H28" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6031,10 +6300,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6188,192 +6457,192 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B8">
         <v>9990180164</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D8" t="s">
         <v>358</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>359</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>360</v>
-      </c>
-      <c r="F8" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B9">
         <v>9411889405</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D9" t="s">
         <v>408</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>409</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>410</v>
-      </c>
-      <c r="F9" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B10">
         <v>9555433468</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="D10" t="s">
         <v>441</v>
       </c>
-      <c r="D10" t="s">
-        <v>442</v>
-      </c>
       <c r="E10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B11">
         <v>9654818693</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" t="s">
+        <v>450</v>
+      </c>
+      <c r="E11" t="s">
         <v>444</v>
-      </c>
-      <c r="D11" t="s">
-        <v>451</v>
-      </c>
-      <c r="E11" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B12">
         <v>9891358561</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D12" t="s">
         <v>464</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>465</v>
-      </c>
-      <c r="E12" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B13">
         <v>8765633150</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B14">
         <v>9990036755</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="D14" t="s">
         <v>491</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>492</v>
-      </c>
-      <c r="E14" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B15">
         <v>9540424976</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D15" t="s">
+        <v>491</v>
+      </c>
+      <c r="E15" t="s">
         <v>492</v>
-      </c>
-      <c r="E15" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B16">
         <v>7042248420</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D16" t="s">
         <v>513</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>514</v>
-      </c>
-      <c r="E16" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B17">
         <v>9911430369</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D17" t="s">
         <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B18">
         <v>8130283991</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="D18" t="s">
         <v>588</v>
-      </c>
-      <c r="D18" t="s">
-        <v>589</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -6381,16 +6650,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B19">
         <v>9565656535</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="D19" t="s">
         <v>597</v>
-      </c>
-      <c r="D19" t="s">
-        <v>598</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -6398,16 +6667,67 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B20">
         <v>9958940360</v>
       </c>
       <c r="D20" t="s">
+        <v>607</v>
+      </c>
+      <c r="E20" t="s">
         <v>608</v>
       </c>
-      <c r="E20" t="s">
-        <v>609</v>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>623</v>
+      </c>
+      <c r="B21">
+        <v>9999518201</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="D21" t="s">
+        <v>588</v>
+      </c>
+      <c r="E21" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>625</v>
+      </c>
+      <c r="B22">
+        <v>8750546916</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="D22" t="s">
+        <v>627</v>
+      </c>
+      <c r="E22" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>629</v>
+      </c>
+      <c r="B23">
+        <v>8285771212</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="D23" t="s">
+        <v>588</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -6430,6 +6750,9 @@
     <hyperlink ref="C17" r:id="rId16"/>
     <hyperlink ref="C18" r:id="rId17"/>
     <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C21" r:id="rId19"/>
+    <hyperlink ref="C22" r:id="rId20"/>
+    <hyperlink ref="C23" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6440,7 +6763,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6454,223 +6777,223 @@
   <sheetData>
     <row r="1" spans="1:5" s="54" customFormat="1">
       <c r="A1" s="85" t="s">
+        <v>558</v>
+      </c>
+      <c r="B1" s="86" t="s">
         <v>559</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="C1" s="86" t="s">
         <v>560</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="D1" s="86" t="s">
         <v>561</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="E1" s="85" t="s">
         <v>562</v>
-      </c>
-      <c r="E1" s="85" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="87" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2" s="88" t="s">
         <v>564</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="C2" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="D2" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="C2" s="88" t="s">
-        <v>565</v>
-      </c>
-      <c r="D2" s="88" t="s">
-        <v>566</v>
-      </c>
       <c r="E2" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="87" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B3" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C3" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="C3" s="88" t="s">
-        <v>566</v>
-      </c>
       <c r="D3" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E3" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="87" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B4" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C4" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="C4" s="88" t="s">
-        <v>566</v>
-      </c>
       <c r="D4" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E4" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45">
       <c r="A5" s="87" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C5" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="D5" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="E5" s="88" t="s">
         <v>565</v>
-      </c>
-      <c r="D5" s="88" t="s">
-        <v>565</v>
-      </c>
-      <c r="E5" s="88" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45">
       <c r="A6" s="87" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C6" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="E6" s="88" t="s">
         <v>565</v>
-      </c>
-      <c r="D6" s="88" t="s">
-        <v>565</v>
-      </c>
-      <c r="E6" s="88" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
       <c r="A7" s="87" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C7" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D7" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E7" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
       <c r="A8" s="87" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D8" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E8" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="87" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B9" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C9" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="C9" s="88" t="s">
-        <v>566</v>
-      </c>
       <c r="D9" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E9" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="87" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B10" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C10" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="C10" s="88" t="s">
-        <v>566</v>
-      </c>
       <c r="D10" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E10" s="88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="87" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B11" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C11" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="C11" s="88" t="s">
-        <v>566</v>
-      </c>
       <c r="D11" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E11" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="87" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B12" s="88" t="s">
+        <v>564</v>
+      </c>
+      <c r="C12" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="C12" s="88" t="s">
-        <v>566</v>
-      </c>
       <c r="D12" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E12" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30">
       <c r="A13" s="87" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B13" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C13" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D13" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E13" s="88" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -6681,10 +7004,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6699,30 +7022,30 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B1" s="81" t="s">
         <v>504</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="C1" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" s="82" t="s">
         <v>505</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="54" t="s">
         <v>509</v>
       </c>
-      <c r="D1" s="82" t="s">
-        <v>506</v>
-      </c>
-      <c r="E1" s="54" t="s">
+      <c r="F1" s="83" t="s">
         <v>510</v>
-      </c>
-      <c r="F1" s="83" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B2" t="s">
         <v>507</v>
-      </c>
-      <c r="B2" t="s">
-        <v>508</v>
       </c>
       <c r="C2">
         <v>31253</v>
@@ -6739,7 +7062,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C3">
         <v>3080</v>
@@ -6753,7 +7076,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C4">
         <v>5000</v>
@@ -6767,7 +7090,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C5">
         <v>1000</v>
@@ -6784,7 +7107,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -6798,7 +7121,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -6812,7 +7135,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C8">
         <v>2300</v>
@@ -6829,7 +7152,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C9">
         <v>1000</v>
@@ -6843,7 +7166,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C10">
         <v>1500</v>
@@ -6860,7 +7183,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C11">
         <v>200</v>
@@ -6874,7 +7197,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C12">
         <v>1400</v>
@@ -6884,6 +7207,20 @@
       </c>
       <c r="F12">
         <v>2435</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>649</v>
+      </c>
+      <c r="C13">
+        <v>2050</v>
+      </c>
+      <c r="E13">
+        <v>4464</v>
+      </c>
+      <c r="F13">
+        <v>4485</v>
       </c>
     </row>
   </sheetData>
@@ -6895,7 +7232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -6916,7 +7253,7 @@
         <v>57</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6965,10 +7302,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" t="s">
         <v>338</v>
-      </c>
-      <c r="B6" t="s">
-        <v>339</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -6976,10 +7313,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C7">
         <v>40</v>
@@ -6987,10 +7324,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -6998,10 +7335,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -7009,10 +7346,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -7020,10 +7357,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C11">
         <v>30</v>
@@ -7031,7 +7368,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B12" t="s">
         <v>67</v>
@@ -7042,10 +7379,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>425</v>
+      </c>
+      <c r="B13" t="s">
         <v>426</v>
-      </c>
-      <c r="B13" t="s">
-        <v>427</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -7053,10 +7390,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>435</v>
+      </c>
+      <c r="B14" t="s">
         <v>436</v>
-      </c>
-      <c r="B14" t="s">
-        <v>437</v>
       </c>
       <c r="C14">
         <v>1000</v>
@@ -7064,10 +7401,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C15">
         <v>105</v>
@@ -7075,10 +7412,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -7086,7 +7423,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
@@ -7097,10 +7434,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>446</v>
+      </c>
+      <c r="B18" t="s">
         <v>447</v>
-      </c>
-      <c r="B18" t="s">
-        <v>448</v>
       </c>
       <c r="C18">
         <v>500</v>
@@ -7108,10 +7445,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>485</v>
+      </c>
+      <c r="B19" t="s">
         <v>486</v>
-      </c>
-      <c r="B19" t="s">
-        <v>487</v>
       </c>
       <c r="C19">
         <v>1200</v>
@@ -7119,10 +7456,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C20">
         <v>500</v>
@@ -7130,10 +7467,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>495</v>
+      </c>
+      <c r="B21" t="s">
         <v>496</v>
-      </c>
-      <c r="B21" t="s">
-        <v>497</v>
       </c>
       <c r="C21">
         <v>300</v>
@@ -7141,10 +7478,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B22" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C22">
         <v>100</v>
@@ -7152,10 +7489,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B23" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C23">
         <v>50</v>
@@ -7163,10 +7500,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B24" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C24">
         <v>10000</v>
@@ -7174,10 +7511,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>540</v>
+      </c>
+      <c r="B25" t="s">
         <v>541</v>
-      </c>
-      <c r="B25" t="s">
-        <v>542</v>
       </c>
       <c r="C25">
         <v>25</v>
@@ -7185,10 +7522,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B26" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C26">
         <v>700</v>
@@ -7196,10 +7533,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>589</v>
+      </c>
+      <c r="B27" t="s">
         <v>590</v>
-      </c>
-      <c r="B27" t="s">
-        <v>591</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -7207,10 +7544,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C28">
         <v>4500</v>
@@ -7223,10 +7560,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7276,177 +7613,185 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>632</v>
       </c>
       <c r="B6">
-        <v>450</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>631</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8">
-        <v>180</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9">
-        <v>250</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10">
-        <v>60</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11">
-        <v>300</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B12">
-        <v>150</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B13">
-        <v>220</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>345</v>
+        <v>87</v>
       </c>
       <c r="B14">
-        <v>750</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>750</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B16">
-        <v>380</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B17">
-        <v>150</v>
+        <v>380</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B18">
-        <v>300</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B19">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B20">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B21">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B22">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B23">
-        <v>800</v>
+        <v>600</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>388</v>
       </c>
       <c r="B24">
-        <v>230</v>
+        <v>800</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>458</v>
+        <v>80</v>
       </c>
       <c r="B25">
-        <v>1250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B26">
-        <v>1450</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B27">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>459</v>
+      </c>
+      <c r="B28">
         <v>1100</v>
       </c>
     </row>
@@ -8176,34 +8521,34 @@
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1" ht="25.5">
       <c r="A1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>36</v>
@@ -8216,13 +8561,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="74" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="75">
         <v>41907</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="77"/>
       <c r="F3" s="74"/>
@@ -8233,11 +8578,11 @@
         <v>6000</v>
       </c>
       <c r="I3" s="73" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J3" s="73"/>
       <c r="K3" s="77" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L3" s="78"/>
     </row>
@@ -8246,17 +8591,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="58">
         <v>41924</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="61">
         <v>9999405538</v>
@@ -8269,7 +8614,7 @@
       </c>
       <c r="J4" s="56"/>
       <c r="K4" s="60" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L4" s="62"/>
     </row>
@@ -8278,17 +8623,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="26">
         <v>41947</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="29">
         <v>9650182218</v>
@@ -8301,7 +8646,7 @@
       </c>
       <c r="J5" s="24"/>
       <c r="K5" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L5" s="31"/>
     </row>
@@ -8310,13 +8655,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="18">
         <v>41947</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="21" t="s">
@@ -8333,7 +8678,7 @@
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L6" s="22"/>
     </row>
@@ -8342,17 +8687,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="26">
         <v>41907</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="29">
         <v>9891085793</v>
@@ -8365,7 +8710,7 @@
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L7" s="31"/>
     </row>
@@ -8374,17 +8719,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="26">
         <v>41947</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="29">
         <v>9350215064</v>
@@ -8397,7 +8742,7 @@
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L8" s="31"/>
     </row>
@@ -8406,13 +8751,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="26">
         <v>41952</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="29"/>
@@ -8427,7 +8772,7 @@
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="28" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L9" s="31"/>
     </row>
@@ -8436,13 +8781,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="26">
         <v>41964</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="29"/>
@@ -8457,7 +8802,7 @@
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L10" s="31"/>
     </row>
@@ -8466,17 +8811,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="26">
         <v>41964</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G11" s="29">
         <v>9958911395</v>
@@ -8491,7 +8836,7 @@
         <v>41971</v>
       </c>
       <c r="K11" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L11" s="31"/>
     </row>
@@ -8500,17 +8845,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="18">
         <v>41964</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>125</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>126</v>
       </c>
       <c r="G12" s="21">
         <v>8527336673</v>
@@ -8523,7 +8868,7 @@
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L12" s="22"/>
     </row>
@@ -8532,13 +8877,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="101" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="102">
         <v>41947</v>
       </c>
       <c r="D13" s="103" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13" s="104"/>
       <c r="F13" s="101" t="s">
@@ -8555,7 +8900,7 @@
       </c>
       <c r="J13" s="100"/>
       <c r="K13" s="104" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L13" s="105"/>
     </row>
@@ -8564,22 +8909,22 @@
         <v>12</v>
       </c>
       <c r="B14" s="93" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="94">
         <v>41947</v>
       </c>
       <c r="D14" s="95" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="99" t="s">
+        <v>603</v>
+      </c>
+      <c r="F14" s="93" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="99" t="s">
-        <v>604</v>
-      </c>
-      <c r="F14" s="93" t="s">
-        <v>132</v>
-      </c>
       <c r="G14" s="93" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H14" s="92">
         <v>10000</v>
@@ -8588,10 +8933,10 @@
         <v>1500</v>
       </c>
       <c r="J14" s="92" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="K14" s="96" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="L14" s="97"/>
     </row>
@@ -8600,16 +8945,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" s="18">
         <v>41983</v>
       </c>
       <c r="D15" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>134</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>135</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21">
@@ -8623,7 +8968,7 @@
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="60" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L15" s="22"/>
     </row>
@@ -8632,13 +8977,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="26">
         <v>41980</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
@@ -8651,7 +8996,7 @@
       </c>
       <c r="J16" s="24"/>
       <c r="K16" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L16" s="31"/>
     </row>
@@ -8660,20 +9005,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C17" s="26">
         <v>41985</v>
       </c>
       <c r="D17" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="35" t="s">
         <v>138</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>139</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H17" s="24">
         <v>5800</v>
@@ -8683,7 +9028,7 @@
       </c>
       <c r="J17" s="24"/>
       <c r="K17" s="30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L17" s="31"/>
     </row>
@@ -8692,22 +9037,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="38">
         <v>41987</v>
       </c>
       <c r="D18" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="F18" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="G18" s="37" t="s">
         <v>143</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="G18" s="37" t="s">
-        <v>144</v>
       </c>
       <c r="H18" s="36">
         <v>4000</v>
@@ -8717,7 +9062,7 @@
       </c>
       <c r="J18" s="36"/>
       <c r="K18" s="30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L18" s="39"/>
     </row>
@@ -8726,20 +9071,20 @@
         <v>19</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="26">
         <v>42020</v>
       </c>
       <c r="D19" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" s="35" t="s">
         <v>146</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>147</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H19" s="24">
         <v>3000</v>
@@ -8749,7 +9094,7 @@
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L19" s="31"/>
     </row>
@@ -8758,22 +9103,22 @@
         <v>20</v>
       </c>
       <c r="B20" s="42" t="s">
+        <v>520</v>
+      </c>
+      <c r="C20" s="41" t="s">
         <v>521</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="D20" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="E20" s="80" t="s">
         <v>523</v>
-      </c>
-      <c r="E20" s="80" t="s">
-        <v>524</v>
       </c>
       <c r="F20" s="42" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H20" s="41">
         <v>5000</v>
@@ -8790,22 +9135,22 @@
         <v>21</v>
       </c>
       <c r="B21" s="42" t="s">
+        <v>530</v>
+      </c>
+      <c r="C21" s="41" t="s">
         <v>531</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="D21" s="42" t="s">
         <v>532</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="E21" s="80" t="s">
         <v>533</v>
       </c>
-      <c r="E21" s="80" t="s">
+      <c r="F21" s="42" t="s">
         <v>534</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="G21" s="42" t="s">
         <v>535</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>536</v>
       </c>
       <c r="H21" s="41">
         <v>3000</v>
@@ -8815,7 +9160,7 @@
       </c>
       <c r="J21" s="41"/>
       <c r="K21" s="43" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="L21" s="44"/>
     </row>
@@ -8824,22 +9169,22 @@
         <v>22</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>580</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="91" t="s">
         <v>582</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>581</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="91" t="s">
+      <c r="F22" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>583</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>584</v>
       </c>
       <c r="H22" s="11">
         <v>3000</v>
@@ -8848,7 +9193,7 @@
         <v>1000</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="38.25">
@@ -8856,22 +9201,22 @@
         <v>23</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>615</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="91" t="s">
         <v>617</v>
       </c>
-      <c r="E23" s="91" t="s">
+      <c r="F23" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>618</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>619</v>
       </c>
       <c r="H23" s="11">
         <v>1000</v>
@@ -8880,7 +9225,7 @@
         <v>6000</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>
@@ -8915,13 +9260,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18">
       <c r="A1" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>153</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="D1" s="15">
         <v>1200</v>
@@ -8935,7 +9280,7 @@
     </row>
     <row r="3" spans="1:4" ht="16.5">
       <c r="A3" s="48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D3" s="15">
         <v>2200</v>
@@ -8943,7 +9288,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="15">
         <v>650</v>
@@ -8954,7 +9299,7 @@
     </row>
     <row r="5" spans="1:4" ht="15">
       <c r="A5" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="15">
         <v>1000</v>
@@ -8965,7 +9310,7 @@
     </row>
     <row r="6" spans="1:4" ht="15">
       <c r="A6" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="15">
         <v>800</v>
@@ -8976,7 +9321,7 @@
     </row>
     <row r="7" spans="1:4" ht="15">
       <c r="A7" s="47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="15">
         <v>975</v>
@@ -8987,7 +9332,7 @@
     </row>
     <row r="8" spans="1:4" ht="15">
       <c r="A8" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="15">
         <v>468</v>
@@ -8998,7 +9343,7 @@
     </row>
     <row r="9" spans="1:4" ht="15">
       <c r="A9" s="47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C9" s="15">
         <v>910</v>
@@ -9009,7 +9354,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="15">
         <v>500</v>
@@ -9020,7 +9365,7 @@
     </row>
     <row r="11" spans="1:4" ht="15">
       <c r="A11" s="47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" s="15">
         <v>800</v>
@@ -9031,7 +9376,7 @@
     </row>
     <row r="12" spans="1:4" ht="15">
       <c r="A12" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="15">
         <v>500</v>
@@ -9042,12 +9387,12 @@
     </row>
     <row r="13" spans="1:4" ht="15">
       <c r="A13" s="50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15">
       <c r="A14" s="47" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C14" s="15">
         <v>975</v>
@@ -9055,7 +9400,7 @@
     </row>
     <row r="15" spans="1:4" ht="15">
       <c r="A15" s="47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="15">
         <v>400</v>
@@ -9063,7 +9408,7 @@
     </row>
     <row r="16" spans="1:4" ht="15">
       <c r="A16" s="47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" s="15">
         <v>910</v>
@@ -9071,12 +9416,12 @@
     </row>
     <row r="17" spans="1:3" ht="15">
       <c r="A17" s="50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="15">
         <v>910</v>
@@ -9084,7 +9429,7 @@
     </row>
     <row r="19" spans="1:3" ht="15">
       <c r="A19" s="47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="15">
         <v>500</v>
@@ -9092,7 +9437,7 @@
     </row>
     <row r="20" spans="1:3" ht="15">
       <c r="A20" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="15">
         <v>450</v>
@@ -9100,7 +9445,7 @@
     </row>
     <row r="21" spans="1:3" ht="15">
       <c r="A21" s="47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="15">
         <v>670</v>
@@ -9108,7 +9453,7 @@
     </row>
     <row r="22" spans="1:3" ht="15">
       <c r="A22" s="47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="15">
         <v>680</v>
@@ -9116,7 +9461,7 @@
     </row>
     <row r="23" spans="1:3" ht="15">
       <c r="A23" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="15">
         <v>780</v>
@@ -9124,7 +9469,7 @@
     </row>
     <row r="24" spans="1:3" ht="15">
       <c r="A24" s="47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="15">
         <v>975</v>
@@ -9132,7 +9477,7 @@
     </row>
     <row r="25" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A25" s="66" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C25" s="10">
         <v>546</v>
@@ -9140,7 +9485,7 @@
     </row>
     <row r="26" spans="1:3" ht="15">
       <c r="A26" s="47" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C26" s="15">
         <v>1820</v>
@@ -9148,7 +9493,7 @@
     </row>
     <row r="27" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A27" s="66" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C27" s="10">
         <v>2041</v>
@@ -9156,7 +9501,7 @@
     </row>
     <row r="28" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A28" s="66" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C28" s="10">
         <v>1040</v>
@@ -9164,7 +9509,7 @@
     </row>
     <row r="29" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A29" s="66" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C29" s="10">
         <v>1000</v>
@@ -9172,7 +9517,7 @@
     </row>
     <row r="30" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A30" s="66" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C30" s="10">
         <v>1950</v>
@@ -9180,17 +9525,17 @@
     </row>
     <row r="31" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A31" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A32" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A33" s="50" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C33" s="55">
         <v>650</v>
@@ -9198,7 +9543,7 @@
     </row>
     <row r="34" spans="1:3" ht="15">
       <c r="A34" s="47" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C34" s="15">
         <v>682</v>
@@ -9206,17 +9551,17 @@
     </row>
     <row r="35" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A35" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A36" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15">
       <c r="A37" s="47" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C37" s="15">
         <v>1079</v>
@@ -9224,7 +9569,7 @@
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="A38" s="47" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C38" s="15">
         <v>780</v>
@@ -9232,7 +9577,7 @@
     </row>
     <row r="39" spans="1:3" ht="15">
       <c r="A39" s="47" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C39" s="15">
         <v>1235</v>
@@ -9240,7 +9585,7 @@
     </row>
     <row r="40" spans="1:3" ht="15">
       <c r="A40" s="47" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C40" s="15">
         <v>500</v>
@@ -9248,7 +9593,7 @@
     </row>
     <row r="41" spans="1:3" ht="15">
       <c r="A41" s="47" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C41" s="15">
         <v>1365</v>
@@ -9256,7 +9601,7 @@
     </row>
     <row r="42" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A42" s="66" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C42" s="10">
         <v>2365</v>
@@ -9264,12 +9609,12 @@
     </row>
     <row r="43" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A43" s="50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="10" customFormat="1" ht="15">
       <c r="A44" s="66" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C44" s="10">
         <v>665</v>
@@ -9277,7 +9622,7 @@
     </row>
     <row r="45" spans="1:3" ht="15">
       <c r="A45" s="47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C45" s="15">
         <v>936</v>
@@ -9285,12 +9630,12 @@
     </row>
     <row r="46" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A46" s="50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15">
       <c r="A47" s="47" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C47" s="15">
         <v>575</v>
@@ -9304,122 +9649,122 @@
     </row>
     <row r="50" spans="1:1" ht="16.5">
       <c r="A50" s="48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15">
       <c r="A51" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15">
       <c r="A52" s="47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15">
       <c r="A53" s="47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15">
       <c r="A54" s="47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15">
       <c r="A55" s="47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15">
       <c r="A56" s="47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15">
       <c r="A57" s="47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15">
       <c r="A58" s="47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15">
       <c r="A59" s="47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15">
       <c r="A60" s="47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15">
       <c r="A61" s="47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15">
       <c r="A62" s="47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15">
       <c r="A63" s="47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15">
       <c r="A64" s="47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15">
       <c r="A65" s="47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15">
       <c r="A66" s="47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15">
       <c r="A67" s="47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15">
       <c r="A68" s="47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15">
       <c r="A69" s="47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15">
       <c r="A70" s="47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15">
       <c r="A71" s="47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15">
       <c r="A72" s="47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15">
       <c r="A73" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15">
@@ -9427,12 +9772,12 @@
     </row>
     <row r="75" spans="1:3" ht="16.5">
       <c r="A75" s="48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15">
       <c r="A76" s="47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C76" s="15">
         <v>1274</v>
@@ -9440,7 +9785,7 @@
     </row>
     <row r="77" spans="1:3" ht="15">
       <c r="A77" s="47" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C77" s="15">
         <v>780</v>
@@ -9448,7 +9793,7 @@
     </row>
     <row r="78" spans="1:3" ht="15">
       <c r="A78" s="47" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C78" s="15">
         <v>910</v>
@@ -9456,7 +9801,7 @@
     </row>
     <row r="79" spans="1:3" ht="15">
       <c r="A79" s="47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C79" s="15">
         <v>1274</v>
@@ -9464,7 +9809,7 @@
     </row>
     <row r="80" spans="1:3" ht="15">
       <c r="A80" s="47" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C80" s="15">
         <v>1066</v>
@@ -9472,7 +9817,7 @@
     </row>
     <row r="81" spans="1:3" ht="15">
       <c r="A81" s="47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C81" s="15">
         <v>1196</v>
@@ -9480,7 +9825,7 @@
     </row>
     <row r="82" spans="1:3" ht="15">
       <c r="A82" s="47" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C82" s="15">
         <v>1196</v>
@@ -9488,7 +9833,7 @@
     </row>
     <row r="83" spans="1:3" ht="15">
       <c r="A83" s="47" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C83" s="15">
         <v>936</v>
@@ -9496,12 +9841,12 @@
     </row>
     <row r="84" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A84" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15">
       <c r="A85" s="47" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C85" s="15">
         <v>975</v>
@@ -9509,12 +9854,12 @@
     </row>
     <row r="86" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A86" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15">
       <c r="A87" s="47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C87" s="15">
         <v>1430</v>
@@ -9522,7 +9867,7 @@
     </row>
     <row r="88" spans="1:3" ht="15">
       <c r="A88" s="47" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C88" s="15">
         <v>1040</v>
@@ -9530,7 +9875,7 @@
     </row>
     <row r="89" spans="1:3" ht="15">
       <c r="A89" s="47" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C89" s="15">
         <v>975</v>
@@ -9538,7 +9883,7 @@
     </row>
     <row r="90" spans="1:3" ht="15">
       <c r="A90" s="47" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C90" s="15">
         <v>1235</v>
@@ -9546,7 +9891,7 @@
     </row>
     <row r="91" spans="1:3" ht="15">
       <c r="A91" s="47" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C91" s="15">
         <v>1430</v>
@@ -9554,7 +9899,7 @@
     </row>
     <row r="92" spans="1:3" ht="15">
       <c r="A92" s="47" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C92" s="15">
         <v>1066</v>
@@ -9562,7 +9907,7 @@
     </row>
     <row r="93" spans="1:3" ht="15">
       <c r="A93" s="47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C93" s="15">
         <v>910</v>
@@ -9570,12 +9915,12 @@
     </row>
     <row r="94" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A94" s="50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15">
       <c r="A95" s="47" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C95" s="15">
         <v>1000</v>
@@ -9583,7 +9928,7 @@
     </row>
     <row r="96" spans="1:3" ht="15">
       <c r="A96" s="47" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C96" s="15">
         <v>1430</v>
@@ -9591,7 +9936,7 @@
     </row>
     <row r="97" spans="1:3" ht="15">
       <c r="A97" s="47" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C97" s="15">
         <v>1065</v>
@@ -9599,12 +9944,12 @@
     </row>
     <row r="98" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A98" s="50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15">
       <c r="A99" s="47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C99" s="15">
         <v>1700</v>
@@ -9612,7 +9957,7 @@
     </row>
     <row r="100" spans="1:3" ht="15">
       <c r="A100" s="47" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C100" s="15">
         <v>3475</v>
@@ -9620,12 +9965,12 @@
     </row>
     <row r="101" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A101" s="50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15">
       <c r="A102" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C102" s="15">
         <v>3035</v>
@@ -9633,7 +9978,7 @@
     </row>
     <row r="103" spans="1:3" ht="15">
       <c r="A103" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15">
@@ -9641,12 +9986,12 @@
     </row>
     <row r="105" spans="1:3" ht="16.5">
       <c r="A105" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15">
       <c r="A106" s="47" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C106" s="15">
         <v>975</v>
@@ -9654,7 +9999,7 @@
     </row>
     <row r="107" spans="1:3" ht="15">
       <c r="A107" s="47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C107" s="15">
         <v>665</v>
@@ -9662,7 +10007,7 @@
     </row>
     <row r="108" spans="1:3" ht="15">
       <c r="A108" s="47" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C108" s="15">
         <v>975</v>
@@ -9670,7 +10015,7 @@
     </row>
     <row r="109" spans="1:3" ht="15">
       <c r="A109" s="47" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C109" s="15">
         <v>675</v>
@@ -9678,7 +10023,7 @@
     </row>
     <row r="110" spans="1:3" ht="15">
       <c r="A110" s="47" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C110" s="15">
         <v>975</v>
@@ -9686,7 +10031,7 @@
     </row>
     <row r="111" spans="1:3" ht="15">
       <c r="A111" s="47" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C111" s="15">
         <v>750</v>
@@ -9694,7 +10039,7 @@
     </row>
     <row r="112" spans="1:3" ht="15">
       <c r="A112" s="47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C112" s="15">
         <v>975</v>
@@ -9702,7 +10047,7 @@
     </row>
     <row r="113" spans="1:3" ht="15">
       <c r="A113" s="47" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C113" s="15">
         <v>300</v>
@@ -9710,7 +10055,7 @@
     </row>
     <row r="114" spans="1:3" ht="15">
       <c r="A114" s="47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C114" s="15">
         <v>660</v>
@@ -9718,12 +10063,12 @@
     </row>
     <row r="115" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A115" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="15">
       <c r="A116" s="47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C116" s="15">
         <v>1066</v>
@@ -9731,7 +10076,7 @@
     </row>
     <row r="117" spans="1:3" ht="15">
       <c r="A117" s="47" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C117" s="15">
         <v>1365</v>
@@ -9739,7 +10084,7 @@
     </row>
     <row r="118" spans="1:3" ht="15">
       <c r="A118" s="47" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C118" s="15">
         <v>1846</v>
@@ -9747,7 +10092,7 @@
     </row>
     <row r="119" spans="1:3" ht="15">
       <c r="A119" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="15">
@@ -9755,17 +10100,17 @@
     </row>
     <row r="121" spans="1:3" ht="16.5">
       <c r="A121" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A122" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15">
       <c r="A123" s="47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C123" s="15">
         <v>2340</v>
@@ -9773,7 +10118,7 @@
     </row>
     <row r="124" spans="1:3" ht="15">
       <c r="A124" s="47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C124" s="15">
         <v>2560</v>
@@ -9781,7 +10126,7 @@
     </row>
     <row r="125" spans="1:3" ht="15">
       <c r="A125" s="47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C125" s="15">
         <v>2807</v>
@@ -9789,7 +10134,7 @@
     </row>
     <row r="126" spans="1:3" ht="15">
       <c r="A126" s="47" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C126" s="15">
         <v>2470</v>
@@ -9797,7 +10142,7 @@
     </row>
     <row r="127" spans="1:3" ht="15">
       <c r="A127" s="47" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C127" s="15">
         <v>2067</v>
@@ -9805,37 +10150,37 @@
     </row>
     <row r="128" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A128" s="50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="129" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A129" s="50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A130" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="131" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A131" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="132" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A132" s="50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="133" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A133" s="50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15">
       <c r="A134" s="47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C134" s="15">
         <v>2375</v>
@@ -9843,42 +10188,42 @@
     </row>
     <row r="135" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A135" s="50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="136" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A136" s="50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="137" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A137" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="138" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A138" s="50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="15">
       <c r="A139" s="47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="140" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A140" s="50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="141" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A141" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15">
       <c r="A142" s="47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C142" s="15">
         <v>2240</v>
@@ -9886,7 +10231,7 @@
     </row>
     <row r="143" spans="1:3" ht="15">
       <c r="A143" s="47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C143" s="15">
         <v>2807</v>
@@ -9894,32 +10239,32 @@
     </row>
     <row r="144" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A144" s="50" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="145" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A145" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="146" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A146" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="147" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A147" s="50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="148" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A148" s="50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="149" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A149" s="50" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="15">
@@ -9927,12 +10272,12 @@
     </row>
     <row r="151" spans="1:3" ht="16.5">
       <c r="A151" s="48" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="15">
       <c r="A152" s="47" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C152" s="15">
         <v>1360</v>
@@ -9940,7 +10285,7 @@
     </row>
     <row r="153" spans="1:3" ht="15">
       <c r="A153" s="47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C153" s="15">
         <v>1615</v>
@@ -9948,7 +10293,7 @@
     </row>
     <row r="154" spans="1:3" ht="15">
       <c r="A154" s="47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C154" s="15">
         <v>1460</v>
@@ -9956,7 +10301,7 @@
     </row>
     <row r="155" spans="1:3" ht="15">
       <c r="A155" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C155" s="15">
         <v>3240</v>
@@ -9964,7 +10309,7 @@
     </row>
     <row r="156" spans="1:3" ht="15">
       <c r="A156" s="47" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C156" s="15">
         <v>1680</v>
@@ -9972,7 +10317,7 @@
     </row>
     <row r="157" spans="1:3" ht="15">
       <c r="A157" s="47" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C157" s="15">
         <v>3900</v>
@@ -9980,17 +10325,17 @@
     </row>
     <row r="158" spans="1:3" ht="15">
       <c r="A158" s="47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="16.5">
       <c r="A159" s="48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="15">
       <c r="A160" s="47" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C160" s="15">
         <v>2470</v>
@@ -9998,7 +10343,7 @@
     </row>
     <row r="161" spans="1:3" ht="15">
       <c r="A161" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C161" s="15">
         <v>2375</v>
@@ -10006,17 +10351,17 @@
     </row>
     <row r="162" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A162" s="50" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="163" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A163" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="164" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A164" s="50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C164" s="55">
         <v>3475</v>
@@ -10024,7 +10369,7 @@
     </row>
     <row r="165" spans="1:3" ht="15">
       <c r="A165" s="47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C165" s="15">
         <v>2360</v>
@@ -10032,62 +10377,62 @@
     </row>
     <row r="166" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A166" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="167" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A167" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="168" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A168" s="50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="169" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A169" s="50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="170" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A170" s="50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="171" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A171" s="50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="172" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A172" s="50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="173" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A173" s="50" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="174" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A174" s="50" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="175" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A175" s="50" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="176" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A176" s="50" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="15">
       <c r="A177" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C177" s="15">
         <v>3190</v>
@@ -10095,12 +10440,12 @@
     </row>
     <row r="178" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A178" s="50" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="15">
       <c r="A179" s="47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C179" s="15">
         <v>2170</v>
@@ -10108,7 +10453,7 @@
     </row>
     <row r="180" spans="1:3" ht="15">
       <c r="A180" s="47" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C180" s="15">
         <v>2390</v>
@@ -10116,12 +10461,12 @@
     </row>
     <row r="181" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A181" s="50" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="15">
       <c r="A182" s="47" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C182" s="15">
         <v>2870</v>
@@ -10129,17 +10474,17 @@
     </row>
     <row r="183" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A183" s="50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="184" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A184" s="50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="15">
       <c r="A185" s="47" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C185" s="15">
         <v>2160</v>
@@ -10147,42 +10492,42 @@
     </row>
     <row r="186" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A186" s="50" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="187" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A187" s="50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="188" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A188" s="50" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="189" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A189" s="50" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="190" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A190" s="50" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="191" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A191" s="50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="192" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A192" s="50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="193" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A193" s="50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="15">
@@ -10190,12 +10535,12 @@
     </row>
     <row r="195" spans="1:3" ht="16.5">
       <c r="A195" s="48" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="15">
       <c r="A196" s="47" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C196" s="15">
         <v>4030</v>
@@ -10203,7 +10548,7 @@
     </row>
     <row r="197" spans="1:3" ht="15">
       <c r="A197" s="47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C197" s="15">
         <v>4280</v>
@@ -10211,7 +10556,7 @@
     </row>
     <row r="198" spans="1:3" ht="15">
       <c r="A198" s="47" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C198" s="15">
         <v>3800</v>
@@ -10219,7 +10564,7 @@
     </row>
     <row r="199" spans="1:3" ht="15">
       <c r="A199" s="47" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C199" s="15">
         <v>3670</v>
@@ -10227,7 +10572,7 @@
     </row>
     <row r="200" spans="1:3" ht="15">
       <c r="A200" s="47" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C200" s="15">
         <v>4280</v>
@@ -10235,12 +10580,12 @@
     </row>
     <row r="201" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A201" s="50" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="15">
       <c r="A202" s="47" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C202" s="15">
         <v>3865</v>
@@ -10248,7 +10593,7 @@
     </row>
     <row r="203" spans="1:3" ht="15">
       <c r="A203" s="47" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C203" s="15">
         <v>3790</v>
@@ -10256,7 +10601,7 @@
     </row>
     <row r="204" spans="1:3" ht="15">
       <c r="A204" s="47" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C204" s="15">
         <v>4290</v>
@@ -10267,12 +10612,12 @@
     </row>
     <row r="206" spans="1:3" ht="16.5">
       <c r="A206" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="15">
       <c r="A207" s="47" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C207" s="15">
         <v>3870</v>
@@ -10280,7 +10625,7 @@
     </row>
     <row r="208" spans="1:3" ht="15">
       <c r="A208" s="47" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C208" s="15">
         <v>4800</v>
@@ -10288,7 +10633,7 @@
     </row>
     <row r="209" spans="1:3" ht="15">
       <c r="A209" s="47" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C209" s="15">
         <v>4600</v>
@@ -10296,7 +10641,7 @@
     </row>
     <row r="210" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A210" s="50" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="15">
@@ -10304,17 +10649,17 @@
     </row>
     <row r="212" spans="1:3" ht="16.5">
       <c r="A212" s="48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="15">
       <c r="A213" s="47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="15">
       <c r="A214" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="15">
@@ -10322,12 +10667,12 @@
     </row>
     <row r="216" spans="1:3" ht="16.5">
       <c r="A216" s="48" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="15">
       <c r="A217" s="47" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C217" s="15">
         <v>2650</v>
@@ -10335,12 +10680,12 @@
     </row>
     <row r="218" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A218" s="50" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="15">
       <c r="A219" s="47" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C219" s="15">
         <v>1760</v>
@@ -10348,32 +10693,32 @@
     </row>
     <row r="220" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A220" s="50" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="221" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A221" s="50" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="222" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A222" s="50" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="223" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A223" s="50" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="224" spans="1:3" s="55" customFormat="1" ht="15">
       <c r="A224" s="50" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="225" spans="1:1" s="55" customFormat="1" ht="15">
       <c r="A225" s="50" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="15">
@@ -10381,12 +10726,12 @@
     </row>
     <row r="227" spans="1:1" ht="16.5">
       <c r="A227" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="228" spans="1:1" ht="15">
       <c r="A228" s="47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="229" spans="1:1" ht="15">
@@ -10394,112 +10739,112 @@
     </row>
     <row r="230" spans="1:1" ht="16.5">
       <c r="A230" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="231" spans="1:1" ht="15">
       <c r="A231" s="47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="15">
       <c r="A232" s="47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="234" spans="1:1" ht="16.5">
       <c r="A234" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" s="49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" s="49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" s="49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" s="49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" s="49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" s="49" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="242" spans="1:1" ht="16.5">
       <c r="A242" s="48" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="244" spans="1:1" ht="16.5">
       <c r="A244" s="48" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="246" spans="1:1" ht="16.5">
       <c r="A246" s="48" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" s="52" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" s="52" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" s="52" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" s="52" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" s="52" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" s="53" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" s="52" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" s="52" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" s="52" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>